<commit_message>
adding columnes to excel file
</commit_message>
<xml_diff>
--- a/TestData1.xlsx
+++ b/TestData1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="126">
   <si>
     <t>Shipping_Method</t>
   </si>
@@ -804,7 +804,7 @@
   <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1321,9 +1321,7 @@
       <c r="I4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3">
@@ -1476,9 +1474,7 @@
       <c r="I5" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3">

</xml_diff>